<commit_message>
updated lines of code in report
</commit_message>
<xml_diff>
--- a/results/heston_sl_comparison.xlsx
+++ b/results/heston_sl_comparison.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="15120" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="16050" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -102,9 +102,6 @@
 [lines of code]</t>
   </si>
   <si>
-    <t>Loopy work in progress</t>
-  </si>
-  <si>
     <t>THDL, Visual Pipeline, VHDL, USB</t>
   </si>
   <si>
@@ -236,6 +233,9 @@
   </si>
   <si>
     <t>Date: September 06, 2013</t>
+  </si>
+  <si>
+    <t>Demo work in progress</t>
   </si>
 </sst>
 </file>
@@ -861,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -887,7 +887,7 @@
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -901,7 +901,7 @@
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -927,34 +927,34 @@
     </row>
     <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="30" t="s">
-        <v>56</v>
-      </c>
       <c r="F11" s="33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G11" s="33"/>
       <c r="H11" s="26"/>
     </row>
     <row r="12" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="7">
         <v>142717770.03484321</v>
@@ -966,7 +966,7 @@
         <v>3</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>4</v>
@@ -987,7 +987,7 @@
         <v>6</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F13" s="37" t="s">
         <v>8</v>
@@ -997,7 +997,7 @@
     </row>
     <row r="14" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="57" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="57"/>
       <c r="C14" s="57"/>
@@ -1012,22 +1012,22 @@
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="30" t="s">
-        <v>56</v>
-      </c>
       <c r="F16" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
@@ -1114,7 +1114,7 @@
     </row>
     <row r="21" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21" s="32">
         <v>599247000</v>
@@ -1173,14 +1173,14 @@
     </row>
     <row r="29" spans="1:8" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
     </row>
     <row r="31" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B31" s="27" t="s">
         <v>26</v>
@@ -1190,7 +1190,7 @@
       </c>
       <c r="D31" s="23"/>
       <c r="E31" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
@@ -1198,7 +1198,7 @@
     </row>
     <row r="32" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="11">
         <v>3705</v>
@@ -1207,14 +1207,14 @@
         <v>1330</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="47" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" s="51">
+        <v>33</v>
+      </c>
+      <c r="B33" s="54">
         <v>5280</v>
       </c>
       <c r="C33" s="54">
@@ -1225,15 +1225,15 @@
         <v>25</v>
       </c>
       <c r="G33" s="53" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" s="11">
-        <v>335</v>
+        <v>415</v>
       </c>
       <c r="C34" s="11">
         <v>540</v>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B35" s="28">
         <v>210</v>
@@ -1266,45 +1266,45 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="str">
-        <f>TEXT(B32/B34,"0.0") &amp; " times smaller code for the same functionality"</f>
-        <v>11.1 times smaller code for the same functionality</v>
+        <f>TEXT(B32/B34,"0") &amp; " times smaller code for the same functionality"</f>
+        <v>9 times smaller code for the same functionality</v>
       </c>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
     </row>
     <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="22"/>
       <c r="B43" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="C43" s="23" t="s">
+      <c r="D43" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="E43" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D43" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="E43" s="23" t="s">
-        <v>47</v>
-      </c>
       <c r="F43" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G43" s="26"/>
       <c r="H43" s="22"/>
     </row>
     <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B44" s="49">
         <f>B45+B46+B48</f>
@@ -1325,7 +1325,7 @@
     </row>
     <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B45" s="20">
         <v>4457</v>
@@ -1342,7 +1342,7 @@
     </row>
     <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46" s="20">
         <v>447</v>
@@ -1357,12 +1357,12 @@
         <v>1</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="47" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B47" s="46">
         <v>3611</v>
@@ -1377,12 +1377,12 @@
         <v>35</v>
       </c>
       <c r="F47" s="47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B48" s="25">
         <v>286</v>
@@ -1402,7 +1402,7 @@
     </row>
     <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B49" s="49">
         <f>SUM(B50:B52)</f>
@@ -1423,7 +1423,7 @@
     </row>
     <row r="50" spans="1:8" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B50" s="42">
         <v>4969</v>
@@ -1442,7 +1442,7 @@
     </row>
     <row r="51" spans="1:8" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51" s="39">
         <v>300</v>
@@ -1457,13 +1457,13 @@
         <v>1</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G51" s="10"/>
     </row>
     <row r="52" spans="1:8" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B52" s="25">
         <v>412</v>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated power in comparison
</commit_message>
<xml_diff>
--- a/results/heston_sl_comparison.xlsx
+++ b/results/heston_sl_comparison.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="16050" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="16980" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -245,7 +245,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="##???0.0E+0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -342,15 +342,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -392,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -549,15 +540,12 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="48" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -573,9 +561,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -613,7 +601,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -685,7 +673,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -861,11 +849,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" style="10" customWidth="1"/>
     <col min="2" max="2" width="16.140625" style="10" customWidth="1"/>
@@ -996,18 +984,18 @@
       <c r="H13" s="21"/>
     </row>
     <row r="14" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1117,10 +1105,10 @@
         <v>63</v>
       </c>
       <c r="B21" s="32">
-        <v>599247000</v>
-      </c>
-      <c r="C21" s="56">
-        <v>4.3013734148121899E-9</v>
+        <v>599362000</v>
+      </c>
+      <c r="C21" s="32">
+        <v>4.6169053272968697E-9</v>
       </c>
       <c r="D21" s="28" t="s">
         <v>17</v>
@@ -1162,13 +1150,13 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="str">
         <f>"Zynq "&amp;TEXT(C12/C21,"0.0") &amp; " more power efficient than DATE 2011 Demo"</f>
-        <v>Zynq 57.1 more power efficient than DATE 2011 Demo</v>
+        <v>Zynq 53.2 more power efficient than DATE 2011 Demo</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="str">
         <f>"Zynq "&amp;TEXT(C17/C21,"0.0") &amp; " more power efficient than Intel CPU"</f>
-        <v>Zynq 50.4 more power efficient than Intel CPU</v>
+        <v>Zynq 47.0 more power efficient than Intel CPU</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
started to add ml comparison
</commit_message>
<xml_diff>
--- a/results/heston_sl_comparison.xlsx
+++ b/results/heston_sl_comparison.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="24420" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="29070" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -14,15 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="78">
   <si>
     <t>Repository: git@git.rhrk.uni-kl.de:EIT-Wehn/finance.zynqpricer.hls.git</t>
   </si>
   <si>
     <t>Author: Christian Brugger (brugger@eit.uni-kl.de)</t>
-  </si>
-  <si>
-    <t>Heston Single Level Monte Carlo, 32bit floating point</t>
   </si>
   <si>
     <t>65 nm</t>
@@ -111,10 +108,6 @@
 (efficiency 48 %)</t>
   </si>
   <si>
-    <t>Heston SL, Date 2011 
-(Yvan, Daniel)</t>
-  </si>
-  <si>
     <t>Heston ML, Date 2013 
 (Pedro, Thomas)</t>
   </si>
@@ -167,9 +160,6 @@
     <t>Zynq Implementation</t>
   </si>
   <si>
-    <t>DATE 2011</t>
-  </si>
-  <si>
     <t>ICDF Gauss</t>
   </si>
   <si>
@@ -217,16 +207,7 @@
     <t>New Software C++</t>
   </si>
   <si>
-    <t>DATE 2011 Demo</t>
-  </si>
-  <si>
     <t>Zync Demo</t>
-  </si>
-  <si>
-    <t>Revision: 980629241b7f4648c347902328718a244f7b511f</t>
-  </si>
-  <si>
-    <t>Date: September 06, 2013</t>
   </si>
   <si>
     <t>Demo work in progress</t>
@@ -254,6 +235,31 @@
   </si>
   <si>
     <t>Core 2 Duo + ML507</t>
+  </si>
+  <si>
+    <t>GPU</t>
+  </si>
+  <si>
+    <t>40 nm</t>
+  </si>
+  <si>
+    <t>Nvidia Tesla C2050</t>
+  </si>
+  <si>
+    <t>ReConFig 2011 Demo</t>
+  </si>
+  <si>
+    <t>Heston Classical Monte Carlo, 32bit floating point</t>
+  </si>
+  <si>
+    <t>Heston, ReConFig
+(Yvan, Daniel)</t>
+  </si>
+  <si>
+    <t>Date: March 31, 2014</t>
+  </si>
+  <si>
+    <t>Revision: 3cc17b6fe870b602fdb9b1b9ff03d1ff1906d8e4</t>
   </si>
 </sst>
 </file>
@@ -401,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -558,6 +564,15 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="48" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -619,7 +634,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -715,7 +730,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>(Tabelle1!$A$12:$A$13,Tabelle1!$A$17:$A$21)</c:f>
+              <c:f>(Tabelle1!$A$12:$A$13,Tabelle1!$A$18:$A$22)</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -746,7 +761,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Tabelle1!$B$12:$B$13,Tabelle1!$B$17:$B$21)</c:f>
+              <c:f>(Tabelle1!$B$12:$B$13,Tabelle1!$B$18:$B$22)</c:f>
               <c:numCache>
                 <c:formatCode>##???0.0E+0</c:formatCode>
                 <c:ptCount val="7"/>
@@ -785,11 +800,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="990359824"/>
-        <c:axId val="990360368"/>
+        <c:axId val="196104608"/>
+        <c:axId val="196105168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="990359824"/>
+        <c:axId val="196104608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -829,10 +844,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="990360368"/>
+        <c:crossAx val="196105168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -840,7 +855,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="990360368"/>
+        <c:axId val="196105168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -888,10 +903,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="990359824"/>
+        <c:crossAx val="196104608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -929,7 +944,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -980,6 +995,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1005,7 +1021,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1158,11 +1174,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="990361456"/>
-        <c:axId val="990363088"/>
+        <c:axId val="196107968"/>
+        <c:axId val="196697904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="990361456"/>
+        <c:axId val="196107968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1202,10 +1218,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="990363088"/>
+        <c:crossAx val="196697904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1213,7 +1229,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="990363088"/>
+        <c:axId val="196697904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1261,10 +1277,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="990361456"/>
+        <c:crossAx val="196107968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1278,6 +1294,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1303,7 +1320,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1333,7 +1350,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1384,6 +1401,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1409,7 +1427,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1562,11 +1580,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="765665040"/>
-        <c:axId val="765666672"/>
+        <c:axId val="196701264"/>
+        <c:axId val="196701824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="765665040"/>
+        <c:axId val="196701264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1606,10 +1624,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="765666672"/>
+        <c:crossAx val="196701824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1617,7 +1635,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="765666672"/>
+        <c:axId val="196701824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1665,10 +1683,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="765665040"/>
+        <c:crossAx val="196701264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1682,6 +1700,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1707,7 +1726,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1737,7 +1756,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1788,6 +1807,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1813,7 +1833,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1966,11 +1986,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1021896592"/>
-        <c:axId val="1021897136"/>
+        <c:axId val="196705184"/>
+        <c:axId val="196818400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1021896592"/>
+        <c:axId val="196705184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2010,10 +2030,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1021897136"/>
+        <c:crossAx val="196818400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2021,7 +2041,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1021897136"/>
+        <c:axId val="196818400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2069,10 +2089,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1021896592"/>
+        <c:crossAx val="196705184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2086,6 +2106,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2111,7 +2132,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2141,7 +2162,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2197,6 +2218,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2222,7 +2244,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2375,11 +2397,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1021893872"/>
-        <c:axId val="1021899312"/>
+        <c:axId val="196821760"/>
+        <c:axId val="196822320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1021893872"/>
+        <c:axId val="196821760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2419,10 +2441,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1021899312"/>
+        <c:crossAx val="196822320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2430,7 +2452,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1021899312"/>
+        <c:axId val="196822320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2478,10 +2500,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1021893872"/>
+        <c:crossAx val="196821760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2495,6 +2517,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2520,7 +2543,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2550,7 +2573,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2724,11 +2747,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1021897680"/>
-        <c:axId val="1021899856"/>
+        <c:axId val="196825680"/>
+        <c:axId val="196961840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1021897680"/>
+        <c:axId val="196825680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2768,10 +2791,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1021899856"/>
+        <c:crossAx val="196961840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2779,7 +2802,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1021899856"/>
+        <c:axId val="196961840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2803,7 +2826,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1021897680"/>
+        <c:crossAx val="196825680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2817,6 +2840,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2842,7 +2866,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2872,7 +2896,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2924,7 +2948,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3020,9 +3044,9 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$L$22:$L$28</c:f>
+              <c:f>Tabelle1!$L$23:$L$30</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Laptop + FPGA
 (efficiency 48 %)</c:v>
@@ -3042,7 +3066,7 @@
                 <c:pt idx="5">
                   <c:v>Zynq ARM only</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Zynq FPGA 6x 
 (efficiency 99.9 %)</c:v>
                 </c:pt>
@@ -3051,10 +3075,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$M$22:$M$28</c:f>
+              <c:f>Tabelle1!$M$23:$M$30</c:f>
               <c:numCache>
                 <c:formatCode>##0.0E+0</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>2.455322265625E-7</c:v>
                 </c:pt>
@@ -3073,7 +3097,7 @@
                 <c:pt idx="5">
                   <c:v>1.7618040873854825E-7</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>4.6169053272968697E-9</c:v>
                 </c:pt>
               </c:numCache>
@@ -3090,11 +3114,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1021900944"/>
-        <c:axId val="1021950336"/>
+        <c:axId val="196964640"/>
+        <c:axId val="196965200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1021900944"/>
+        <c:axId val="196964640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3134,10 +3158,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1021950336"/>
+        <c:crossAx val="196965200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3145,7 +3169,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1021950336"/>
+        <c:axId val="196965200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0000000000000004E-6"/>
@@ -3194,10 +3218,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1021900944"/>
+        <c:crossAx val="196964640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3235,7 +3259,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3312,7 +3336,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3352,7 +3376,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$K$32:$K$33</c:f>
+              <c:f>Tabelle1!$K$34:$K$35</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -3366,7 +3390,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$L$32:$L$33</c:f>
+              <c:f>Tabelle1!$L$34:$L$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -3390,11 +3414,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1021949248"/>
-        <c:axId val="1021949792"/>
+        <c:axId val="196967440"/>
+        <c:axId val="196968000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1021949248"/>
+        <c:axId val="196967440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3434,10 +3458,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1021949792"/>
+        <c:crossAx val="196968000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3445,7 +3469,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1021949792"/>
+        <c:axId val="196968000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3493,10 +3517,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1021949248"/>
+        <c:crossAx val="196967440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3534,7 +3558,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7901,7 +7925,7 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8045,7 +8069,7 @@
     <xdr:from>
       <xdr:col>24</xdr:col>
       <xdr:colOff>201083</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>78316</xdr:rowOff>
     </xdr:from>
     <xdr:to>
@@ -8081,7 +8105,7 @@
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>338665</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>6351</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8105,13 +8129,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>534458</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>141817</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>195791</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>91017</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8135,9 +8159,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -8175,7 +8199,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -8247,7 +8271,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8423,8 +8447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -8442,14 +8466,14 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -8463,7 +8487,7 @@
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -8478,7 +8502,7 @@
     <row r="6" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:10" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -8489,34 +8513,34 @@
     </row>
     <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F11" s="33" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G11" s="33"/>
       <c r="H11" s="26"/>
     </row>
     <row r="12" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="7">
         <v>142717770.03484321</v>
@@ -8525,448 +8549,475 @@
         <v>2.455322265625E-7</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="57">
+        <v>62060606.060606062</v>
+      </c>
+      <c r="C13" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="55">
-        <v>62060606.060606062</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="21"/>
+      <c r="E13" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="43"/>
     </row>
-    <row r="14" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="56" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
+    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="55">
+        <v>345800000</v>
+      </c>
+      <c r="C14" s="35">
+        <v>8.9650000000000001E-7</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="37"/>
+      <c r="H14" s="21"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16" s="30" t="s">
+    <row r="15" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
     </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="12">
-        <v>267701000</v>
-      </c>
-      <c r="C17" s="12">
-        <v>6.9480502500924538E-7</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>7</v>
-      </c>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B18" s="12">
-        <v>141086000</v>
+        <v>267701000</v>
       </c>
       <c r="C18" s="12">
-        <v>2.1688898969422907E-7</v>
+        <v>6.9480502500924538E-7</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>73</v>
+        <v>5</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B19" s="12">
-        <v>214878000</v>
+        <v>141086000</v>
       </c>
       <c r="C19" s="12">
-        <v>7.1668574726123663E-7</v>
+        <v>2.1688898969422907E-7</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B20" s="12">
+        <v>214878000</v>
+      </c>
+      <c r="C20" s="12">
+        <v>7.1668574726123663E-7</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="12">
         <v>10784400</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C21" s="12">
         <v>1.7618040873854825E-7</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D21" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="32">
+        <v>599362000</v>
+      </c>
+      <c r="C22" s="32">
+        <v>4.6169053272968697E-9</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="F22" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="10" t="s">
-        <v>19</v>
-      </c>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
     </row>
-    <row r="21" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="32">
-        <v>599362000</v>
-      </c>
-      <c r="C21" s="32">
-        <v>4.6169053272968697E-9</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-    </row>
-    <row r="22" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="L22" s="10" t="str">
+    <row r="23" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="L23" s="10" t="str">
         <f>A12</f>
         <v>Laptop + FPGA
 (efficiency 48 %)</v>
       </c>
-      <c r="M22" s="12">
+      <c r="M23" s="12">
         <f>C12</f>
         <v>2.455322265625E-7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="str">
-        <f>"ARM "&amp;TEXT(C18/C20-1,"0%") &amp; " more power efficient than Intel Laptop"</f>
-        <v>ARM 23% more power efficient than Intel Laptop</v>
-      </c>
-      <c r="C23" s="14"/>
-      <c r="E23" s="15"/>
-      <c r="L23" s="10" t="str">
-        <f>A13</f>
-        <v>Server</v>
-      </c>
-      <c r="M23" s="12">
-        <v>2.9969999999999999E-6</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="str">
-        <f>"Optimized C++ Implementation "&amp;TEXT(B17/B13,"0.0") &amp; " times faster than DATE 2011 implementation (Vectorized (AVX), Cache Optimization, Ziggurat)"</f>
-        <v>Optimized C++ Implementation 4.3 times faster than DATE 2011 implementation (Vectorized (AVX), Cache Optimization, Ziggurat)</v>
-      </c>
+        <f>"ARM "&amp;TEXT(C19/C21-1,"0%") &amp; " more power efficient than Intel Laptop"</f>
+        <v>ARM 23% more power efficient than Intel Laptop</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="E24" s="15"/>
       <c r="L24" s="10" t="str">
-        <f>A17</f>
+        <f>A13</f>
         <v>Server</v>
       </c>
       <c r="M24" s="12">
-        <f>C17</f>
-        <v>6.9480502500924538E-7</v>
+        <v>2.9969999999999999E-6</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="str">
-        <f>"Zynq "&amp;TEXT(B21/B12,"0.0") &amp; " times faster than DATE 2011 Demo"</f>
-        <v>Zynq 4.2 times faster than DATE 2011 Demo</v>
+        <f>"Optimized C++ Implementation "&amp;TEXT(B18/B13,"0.0") &amp; " times faster than ReConFig 2011 implementation (Vectorized, Cache Optimization, Ziggurat)"</f>
+        <v>Optimized C++ Implementation 4.3 times faster than ReConFig 2011 implementation (Vectorized, Cache Optimization, Ziggurat)</v>
       </c>
       <c r="L25" s="10" t="str">
         <f>A18</f>
-        <v>Dell Laptop</v>
+        <v>Server</v>
       </c>
       <c r="M25" s="12">
-        <f t="shared" ref="M25:M28" si="0">C18</f>
-        <v>2.1688898969422907E-7</v>
+        <f>C18</f>
+        <v>6.9480502500924538E-7</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="str">
-        <f>"Zynq "&amp;TEXT(C12/C21,"0.0") &amp; " more power efficient than DATE 2011 Demo"</f>
-        <v>Zynq 53.2 more power efficient than DATE 2011 Demo</v>
+        <f>"Zynq "&amp;TEXT(B22/B12,"0.0") &amp; " times faster than ReConFig 2011 Demo"</f>
+        <v>Zynq 4.2 times faster than ReConFig 2011 Demo</v>
       </c>
       <c r="L26" s="10" t="str">
         <f>A19</f>
-        <v>Dell Desktop</v>
+        <v>Dell Laptop</v>
       </c>
       <c r="M26" s="12">
-        <f t="shared" si="0"/>
-        <v>7.1668574726123663E-7</v>
+        <f t="shared" ref="M26:M28" si="0">C19</f>
+        <v>2.1688898969422907E-7</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="str">
-        <f>"Zynq "&amp;TEXT(C18/C21,"0.0") &amp; " more power efficient than Intel CPU"</f>
-        <v>Zynq 47.0 more power efficient than Intel CPU</v>
+        <f>"Zynq "&amp;TEXT(C12/C22,"0.0") &amp; " more power efficient than ReConFig 2011 Demo"</f>
+        <v>Zynq 53.2 more power efficient than ReConFig 2011 Demo</v>
       </c>
       <c r="L27" s="10" t="str">
         <f>A20</f>
-        <v>Zynq ARM only</v>
+        <v>Dell Desktop</v>
       </c>
       <c r="M27" s="12">
         <f t="shared" si="0"/>
-        <v>1.7618040873854825E-7</v>
+        <v>7.1668574726123663E-7</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="str">
+        <f>"Zynq "&amp;TEXT(C19/C22,"0.0") &amp; " more power efficient than Intel CPU" &amp; " and "&amp;TEXT(C14/C22,"0.0") &amp; " more power efficient than GPU"</f>
+        <v>Zynq 47.0 more power efficient than Intel CPU and 194.2 more power efficient than GPU</v>
+      </c>
       <c r="L28" s="10" t="str">
         <f>A21</f>
+        <v>Zynq ARM only</v>
+      </c>
+      <c r="M28" s="12">
+        <f t="shared" si="0"/>
+        <v>1.7618040873854825E-7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="str">
+        <f>"Zynq "&amp;TEXT(B22/B18,"0.0") &amp; " faster than Intel Server" &amp; " and "&amp;TEXT(B22/B14,"0.0") &amp; " faster than GPU"</f>
+        <v>Zynq 2.2 faster than Intel Server and 1.7 faster than GPU</v>
+      </c>
+      <c r="M29" s="12"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L30" s="10" t="str">
+        <f>A22</f>
         <v>Zynq FPGA 6x 
 (efficiency 99.9 %)</v>
       </c>
-      <c r="M28" s="12">
-        <f t="shared" si="0"/>
+      <c r="M30" s="12">
+        <f>C22</f>
         <v>4.6169053272968697E-9</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
+    <row r="31" spans="1:13" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
     </row>
-    <row r="31" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="B31" s="27" t="s">
+    <row r="33" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-    </row>
-    <row r="32" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="11">
-        <v>3705</v>
-      </c>
-      <c r="C32" s="11">
-        <v>1330</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="K32" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="L32" s="10">
-        <f>B32</f>
-        <v>3705</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" s="47" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="54">
-        <v>5280</v>
-      </c>
-      <c r="C33" s="54">
-        <v>7870</v>
-      </c>
-      <c r="D33" s="51"/>
-      <c r="E33" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="G33" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="K33" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="L33" s="47">
-        <f>B34</f>
-        <v>415</v>
-      </c>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
     </row>
     <row r="34" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
-        <v>32</v>
+      <c r="A34" s="16" t="s">
+        <v>75</v>
       </c>
       <c r="B34" s="11">
+        <v>3705</v>
+      </c>
+      <c r="C34" s="11">
+        <v>1330</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K34" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="L34" s="10">
+        <f>B34</f>
+        <v>3705</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" s="47" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="54">
+        <v>5280</v>
+      </c>
+      <c r="C35" s="54">
+        <v>7870</v>
+      </c>
+      <c r="D35" s="51"/>
+      <c r="E35" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="K35" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="L35" s="47">
+        <f>B36</f>
         <v>415</v>
       </c>
-      <c r="C34" s="11">
+    </row>
+    <row r="36" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="11">
+        <v>415</v>
+      </c>
+      <c r="C36" s="11">
         <v>540</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E36" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" s="28">
+        <v>210</v>
+      </c>
+      <c r="C37" s="28">
+        <v>150</v>
+      </c>
+      <c r="D37" s="28"/>
+      <c r="E37" s="21" t="s">
         <v>21</v>
       </c>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
     </row>
-    <row r="35" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B35" s="28">
-        <v>210</v>
-      </c>
-      <c r="C35" s="28">
-        <v>150</v>
-      </c>
-      <c r="D35" s="28"/>
-      <c r="E35" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="str">
+        <f>TEXT(B34/B36,"0") &amp; " times smaller code for the same functionality"</f>
+        <v>9 times smaller code for the same functionality</v>
+      </c>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="str">
-        <f>TEXT(B32/B34,"0") &amp; " times smaller code for the same functionality"</f>
-        <v>9 times smaller code for the same functionality</v>
-      </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-    </row>
-    <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
-        <v>38</v>
+    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="J42" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K42" s="10" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="L42" s="10" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="N42" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O42" s="10" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="P42" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="S42" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="T42" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="S42" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="T42" s="10" t="s">
-        <v>74</v>
-      </c>
       <c r="U42" s="10" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="22"/>
       <c r="B43" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D43" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="E43" s="23" t="s">
-        <v>44</v>
-      </c>
       <c r="F43" s="26" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G43" s="26"/>
       <c r="H43" s="22"/>
       <c r="J43" s="10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="K43" s="10">
         <f>B49</f>
@@ -8977,7 +9028,7 @@
         <v>5190</v>
       </c>
       <c r="N43" s="10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="O43" s="10">
         <f>C49</f>
@@ -8988,7 +9039,7 @@
         <v>5358</v>
       </c>
       <c r="S43" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="T43" s="10">
         <f>K43</f>
@@ -9001,7 +9052,7 @@
     </row>
     <row r="44" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B44" s="49">
         <f>B45+B46+B48</f>
@@ -9020,7 +9071,7 @@
         <v>36</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="K44" s="10">
         <f>B52</f>
@@ -9031,7 +9082,7 @@
         <v>286</v>
       </c>
       <c r="N44" s="10" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="O44" s="10">
         <f>C52</f>
@@ -9042,7 +9093,7 @@
         <v>323</v>
       </c>
       <c r="S44" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="T44" s="10">
         <f>O43</f>
@@ -9055,7 +9106,7 @@
     </row>
     <row r="45" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B45" s="20">
         <v>4457</v>
@@ -9070,7 +9121,7 @@
         <v>35</v>
       </c>
       <c r="J45" s="10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="K45" s="10">
         <f>B51</f>
@@ -9081,7 +9132,7 @@
         <v>447</v>
       </c>
       <c r="N45" s="10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="O45" s="10">
         <f>C51</f>
@@ -9092,7 +9143,7 @@
         <v>592</v>
       </c>
       <c r="S45" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="T45" s="10">
         <f>K66*1000</f>
@@ -9105,7 +9156,7 @@
     </row>
     <row r="46" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B46" s="20">
         <v>447</v>
@@ -9120,10 +9171,10 @@
         <v>1</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K46" s="10">
         <f>B50</f>
@@ -9134,7 +9185,7 @@
         <v>4457</v>
       </c>
       <c r="N46" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="O46" s="10">
         <f>C50</f>
@@ -9145,7 +9196,7 @@
         <v>4443</v>
       </c>
       <c r="S46" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="T46" s="10">
         <f>O66*100</f>
@@ -9156,9 +9207,9 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="47" spans="1:21" s="47" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:21" s="47" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="45" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B47" s="46">
         <v>3611</v>
@@ -9173,12 +9224,12 @@
         <v>35</v>
       </c>
       <c r="F47" s="47" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B48" s="25">
         <v>286</v>
@@ -9198,7 +9249,7 @@
     </row>
     <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="B49" s="49">
         <f>SUM(B50:B52)</f>
@@ -9219,7 +9270,7 @@
     </row>
     <row r="50" spans="1:8" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="41" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B50" s="42">
         <v>4969</v>
@@ -9238,7 +9289,7 @@
     </row>
     <row r="51" spans="1:8" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="38" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B51" s="39">
         <v>300</v>
@@ -9253,13 +9304,13 @@
         <v>1</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G51" s="10"/>
     </row>
     <row r="52" spans="1:8" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B52" s="25">
         <v>412</v>
@@ -9279,32 +9330,32 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="65" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J65" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K65" s="10" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="L65" s="10" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="N65" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O65" s="10" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="P65" s="10" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J66" s="10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="K66" s="10">
         <f>D49</f>
@@ -9315,7 +9366,7 @@
         <v>5</v>
       </c>
       <c r="N66" s="10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="O66" s="10">
         <f>E49</f>
@@ -9328,7 +9379,7 @@
     </row>
     <row r="67" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J67" s="10" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="K67" s="10">
         <f>D52</f>
@@ -9339,7 +9390,7 @@
         <v>2</v>
       </c>
       <c r="N67" s="10" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="O67" s="10">
         <f>E52</f>
@@ -9352,7 +9403,7 @@
     </row>
     <row r="68" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J68" s="10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="K68" s="10">
         <f t="shared" ref="K68" si="3">D51</f>
@@ -9363,7 +9414,7 @@
         <v>2</v>
       </c>
       <c r="N68" s="10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="O68" s="10">
         <f t="shared" ref="O68" si="5">E51</f>
@@ -9376,7 +9427,7 @@
     </row>
     <row r="69" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J69" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K69" s="10">
         <f>D50</f>
@@ -9387,7 +9438,7 @@
         <v>1</v>
       </c>
       <c r="N69" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="O69" s="10">
         <f>E50</f>
@@ -9400,7 +9451,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A14:J14"/>
+    <mergeCell ref="A15:J15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="85" orientation="portrait" r:id="rId1"/>

</xml_diff>